<commit_message>
Dándole pesos probabilisticos a los productos para apoyar la hipótesis
</commit_message>
<xml_diff>
--- a/Generacion_datos/TP_Final_Especificacion_1.xlsx
+++ b/Generacion_datos/TP_Final_Especificacion_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\OneDrive\Documentos\Mis Archivos\Infraestructura para Ciencia de Datos\TP_Final\Generacion_datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\OneDrive\Documentos\Mis Archivos\Infraestructura para Ciencia de Datos\TP_Final\generacion_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75941DD3-3D90-40E6-BEA2-32390544C31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCFB184-E5E4-4CD5-8B19-DB2CBA57A4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="2115" windowWidth="17130" windowHeight="10395" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Desc_Ventas" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
   <si>
     <t>Campo</t>
   </si>
@@ -15029,65 +15029,100 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>101</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -15102,7 +15137,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Generación de datos para un año
</commit_message>
<xml_diff>
--- a/Generacion_datos/TP_Final_Especificacion_1.xlsx
+++ b/Generacion_datos/TP_Final_Especificacion_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\OneDrive\Documentos\Mis Archivos\Infraestructura para Ciencia de Datos\TP_Final\generacion_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCFB184-E5E4-4CD5-8B19-DB2CBA57A4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C44307-901C-4D3B-AB53-0C4D9A5FB147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Desc_Ventas" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
   <si>
     <t>Campo</t>
   </si>
@@ -456,7 +456,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +501,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -535,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -581,6 +589,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15031,8 +15041,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15114,7 +15124,7 @@
         <v>100</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -15122,7 +15132,7 @@
         <v>101</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -15135,10 +15145,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15148,7 +15158,7 @@
     <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -15164,8 +15174,11 @@
       <c r="E1" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>107</v>
       </c>
@@ -15181,8 +15194,11 @@
       <c r="E2" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>109</v>
       </c>
@@ -15198,8 +15214,11 @@
       <c r="E3" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>114</v>
       </c>
@@ -15215,8 +15234,11 @@
       <c r="E4" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>119</v>
       </c>
@@ -15232,8 +15254,11 @@
       <c r="E5" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>136</v>
       </c>
@@ -15249,9 +15274,16 @@
       <c r="E6" s="3" t="s">
         <v>127</v>
       </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>